<commit_message>
Update excel reporting function
</commit_message>
<xml_diff>
--- a/public/report/Attendance Reporting.xlsx
+++ b/public/report/Attendance Reporting.xlsx
@@ -4,19 +4,223 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="My Sheet" r:id="rId4"/>
+    <sheet sheetId="1" name="Monthly Attendance Reporting" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>Month</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+  <si>
+    <t>Monthly Attendance Reporting: Feb 2018</t>
+  </si>
+  <si>
+    <t>Working Day</t>
+  </si>
+  <si>
+    <t>Month : Feb 2018</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t>Sat</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>TOTAL VISIT</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Blk</t>
+  </si>
+  <si>
+    <t>Unit No</t>
+  </si>
+  <si>
+    <t>Name of Registered Elderly</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>#03-xxx</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Total Attendance for the Day</t>
+  </si>
+  <si>
+    <t>Month : FEB 2018</t>
+  </si>
+  <si>
+    <t>Total # of seniors (est)</t>
+  </si>
+  <si>
+    <t>Total # of members</t>
+  </si>
+  <si>
+    <t>Total attendance for the month</t>
+  </si>
+  <si>
+    <t>No of working days in the month</t>
+  </si>
+  <si>
+    <t>Average daily attendance</t>
+  </si>
+  <si>
+    <t>Total # of active members</t>
+  </si>
+  <si>
+    <t>% of members</t>
+  </si>
+  <si>
+    <t>% of Active members</t>
+  </si>
+  <si>
+    <t>moved out</t>
+  </si>
+  <si>
+    <t>passed away</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Public holiday</t>
+  </si>
+  <si>
+    <t>New Members</t>
+  </si>
+  <si>
+    <t>Not Registered Members</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Centre Closed</t>
   </si>
 </sst>
 </file>
@@ -32,7 +236,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,8 +248,48 @@
         <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB266"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF336600"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,13 +297,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,24 +663,662 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:AM32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="str">
+        <f>=SUM(F6:F10)</f>
+        <v/>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f>=SUM(G6:G10)</f>
+        <v/>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f>=SUM(H6:H10)</f>
+        <v/>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>=SUM(I6:I10)</f>
+        <v/>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f>=SUM(J6:J10)</f>
+        <v/>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f>=SUM(K6:K10)</f>
+        <v/>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f>=SUM(L6:L10)</f>
+        <v/>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f>=SUM(M6:M10)</f>
+        <v/>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f>=SUM(N6:N10)</f>
+        <v/>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f>=SUM(O6:O10)</f>
+        <v/>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f>=SUM(P6:P10)</f>
+        <v/>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f>=SUM(Q6:Q10)</f>
+        <v/>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f>=SUM(R6:R10)</f>
+        <v/>
+      </c>
+      <c r="S10" s="1" t="str">
+        <f>=SUM(S6:S10)</f>
+        <v/>
+      </c>
+      <c r="T10" s="1" t="str">
+        <f>=SUM(T6:T10)</f>
+        <v/>
+      </c>
+      <c r="U10" s="1" t="str">
+        <f>=SUM(U6:U10)</f>
+        <v/>
+      </c>
+      <c r="V10" s="1" t="str">
+        <f>=SUM(V6:V10)</f>
+        <v/>
+      </c>
+      <c r="W10" s="1" t="str">
+        <f>=SUM(W6:W10)</f>
+        <v/>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f>=SUM(X6:X10)</f>
+        <v/>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f>=SUM(Y6:Y10)</f>
+        <v/>
+      </c>
+      <c r="Z10" s="1" t="str">
+        <f>=SUM(Z6:Z10)</f>
+        <v/>
+      </c>
+      <c r="AA10" s="1" t="str">
+        <f>=SUM(AA6:AA10)</f>
+        <v/>
+      </c>
+      <c r="AB10" s="1" t="str">
+        <f>=SUM(AB6:AB10)</f>
+        <v/>
+      </c>
+      <c r="AC10" s="1" t="str">
+        <f>=SUM(AC6:AC10)</f>
+        <v/>
+      </c>
+      <c r="AD10" s="1" t="str">
+        <f>=SUM(AD6:AD10)</f>
+        <v/>
+      </c>
+      <c r="AE10" s="1" t="str">
+        <f>=SUM(AE6:AE10)</f>
+        <v/>
+      </c>
+      <c r="AF10" s="1" t="str">
+        <f>=SUM(AF6:AF10)</f>
+        <v/>
+      </c>
+      <c r="AG10" s="1" t="str">
+        <f>=SUM(AG6:AG10)</f>
+        <v/>
+      </c>
+      <c r="AH10" s="1" t="str">
+        <f>=SUM(AH6:AH10)</f>
+        <v/>
+      </c>
+      <c r="AI10" s="1" t="str">
+        <f>=SUM(AI6:AI10)</f>
+        <v/>
+      </c>
+      <c r="AJ10" s="1" t="str">
+        <f>=SUM(AJ6:AJ10)</f>
+        <v/>
+      </c>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="E27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="8"/>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="E29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="10"/>
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="12"/>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A4:C4"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>